<commit_message>
reverted to for-test-only dataToFile; editted instuctors sample files
</commit_message>
<xml_diff>
--- a/frontend/src/tests/samples/instructors.xlsx
+++ b/frontend/src/tests/samples/instructors.xlsx
@@ -1,110 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="480" yWindow="48" windowWidth="22056" windowHeight="9696"/>
-  </bookViews>
+  <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Instructors" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
-  <si>
-    <t>Last Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>First Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UTORid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>email</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gordon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Smith</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>booger</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a@a.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tommy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>food</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a@b.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fooc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Boobie</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Grandpa</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a@d.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -125,38 +39,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -300,20 +198,16 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -435,113 +329,116 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="11.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Last Name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>First Name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>UTORid</v>
+      </c>
+      <c r="D1" t="str">
+        <v>email</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Smith</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Henry</v>
+      </c>
+      <c r="C2" t="str">
+        <v>smithh</v>
+      </c>
+      <c r="D2" t="str">
+        <v>hery.smith@utoronto.ca</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Garcia</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Emily</v>
+      </c>
+      <c r="C3" t="str">
+        <v>garciae</v>
+      </c>
+      <c r="D3" t="str">
+        <v>emily.garcia@utoronto.ca</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Miller</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Megan</v>
+      </c>
+      <c r="C4" t="str">
+        <v>millerm</v>
+      </c>
+      <c r="D4" t="str">
+        <v>megan.miller@utoronto.ca</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>